<commit_message>
Test Results and classification
</commit_message>
<xml_diff>
--- a/January 2023 Analysis/New Analysis/3-section-separate/sampleset/Results/Exp 13 Result 13.xlsx
+++ b/January 2023 Analysis/New Analysis/3-section-separate/sampleset/Results/Exp 13 Result 13.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rashedhasan/Desktop/UNL/Research/Object relational mapping/Step 5 - Abstraction/OM-Solution_Mapping/OM-ML_Research/January 2023 Analysis/New Analysis/3-section-separate/sampleset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rashedhasan/Desktop/UNL/Research/Object relational mapping/Step 5 - Abstraction/OM-Solution_Mapping/OM-ML_Research/January 2023 Analysis/New Analysis/3-section-separate/sampleset/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD77FC09-E41F-7B46-979C-7993AB866D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697FC5F5-F49E-8D4F-A74D-F5BC09B07F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{9E606C90-6937-7643-AC22-ADE071A6A0E2}"/>
+    <workbookView xWindow="4560" yWindow="2520" windowWidth="28040" windowHeight="16380" xr2:uid="{9E606C90-6937-7643-AC22-ADE071A6A0E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -345,7 +345,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -372,6 +372,11 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -393,11 +398,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE80F2C-09A0-644A-8168-23135C5417CA}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,18 +732,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="1"/>
@@ -748,13 +755,13 @@
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B6" s="1"/>
@@ -772,7 +779,7 @@
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="1"/>
@@ -820,7 +827,7 @@
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B17" s="1"/>
@@ -862,7 +869,7 @@
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B24" s="2"/>
@@ -952,13 +959,13 @@
       <c r="B38" s="2"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B39" s="1"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B40" s="1"/>
@@ -982,7 +989,7 @@
       <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B44" s="1"/>
@@ -994,7 +1001,7 @@
       <c r="B45" s="2"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="1"/>
@@ -1060,7 +1067,7 @@
       <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B57" s="1"/>
@@ -1090,7 +1097,7 @@
       <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B62" s="1"/>
@@ -1144,163 +1151,163 @@
       <c r="B70" s="2"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B71" s="2"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B72" s="2"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B73" s="2"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B74" s="2"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B75" s="2"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="2"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B77" s="2"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B78" s="1"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B79" s="2"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B80" s="2"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B81" s="2"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B82" s="2"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B83" s="2"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B84" s="2"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B85" s="2"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B86" s="2"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B87" s="2"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B88" s="1"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B89" s="2"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B90" s="2"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B91" s="2"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B92" s="2"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B93" s="2"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B94" s="2"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B95" s="2"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B96" s="2"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B97" s="2"/>
@@ -1312,19 +1319,19 @@
       <c r="B98" s="1"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B99" s="2"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B100" s="2"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B101" s="2"/>

</xml_diff>